<commit_message>
Docs updated with testcases
</commit_message>
<xml_diff>
--- a/Docs/Teszt.xlsx
+++ b/Docs/Teszt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
   <si>
     <t>Folyamat</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Felhasználónév</t>
   </si>
   <si>
-    <t>Sikeres bejelentkezés</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Elvárt</t>
   </si>
   <si>
-    <t>Sikeres bejelentkezés után látható 3 fül a navigációban. Az alapértelmezett fül tartalmazza a rögzített tárgyak listáját, megjelennek a gombok a lista fölött: Hozzáadás, Szűrők törlése, Törlés (inaktív), Áthelyezés (inaktív) lista alatt: Műveleti Napló Letöltése, Címkék Letöltése. Látható a tárgyak és termek kezelése.</t>
-  </si>
-  <si>
     <t>Tároló rögzítés</t>
   </si>
   <si>
@@ -68,12 +62,6 @@
     <t>Tároló név</t>
   </si>
   <si>
-    <t>Sikeres tároló rögzítés</t>
-  </si>
-  <si>
-    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on, a listában kiíródik az új tároló.</t>
-  </si>
-  <si>
     <t>Tároló törlése</t>
   </si>
   <si>
@@ -84,13 +72,250 @@
   </si>
   <si>
     <t>A listában szereplő adatok mellett található törlés gomb biztosítja az egyedi törlést.</t>
+  </si>
+  <si>
+    <t>Tárgy név</t>
+  </si>
+  <si>
+    <t>Teszt tárgy</t>
+  </si>
+  <si>
+    <t>Egyedi tárgy rögzítése</t>
+  </si>
+  <si>
+    <t>Mennyiség</t>
+  </si>
+  <si>
+    <t>Tárgynév</t>
+  </si>
+  <si>
+    <t>Tárolónév</t>
+  </si>
+  <si>
+    <t>Tárgynév rögzítés</t>
+  </si>
+  <si>
+    <t>Egyedi tárgy törlése</t>
+  </si>
+  <si>
+    <t>Egyedi tárgy áthelyezése</t>
+  </si>
+  <si>
+    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on "A termék sikeresen hozzáadva!". A listában kiíródik az új tárgy.</t>
+  </si>
+  <si>
+    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on "A raktár törlése sikeres!". A listában kiíródik az új tároló.</t>
+  </si>
+  <si>
+    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on "A termék törlése sikeres!". A listában kiíródik az új tárgy.</t>
+  </si>
+  <si>
+    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on "A raktár sikeresen hozzáadva!".  A listában kiíródik az új tároló.</t>
+  </si>
+  <si>
+    <t>Tárgynevet törlése, míg rögzített egyedi tárgyak használják a tárgynevet</t>
+  </si>
+  <si>
+    <t>Tároló törlése, míg rögzített egyedi tárgyak használják a tárolót</t>
+  </si>
+  <si>
+    <t>Tárgynév törlése</t>
+  </si>
+  <si>
+    <t>Megfelelő hibaüzenet jelenik meg a UI-on " A raktár törlése sikertelen! Ellenőrizze, hogy nincs-e termék a raktárban!".</t>
+  </si>
+  <si>
+    <t>Megfelelő hibaüzenet jelenik meg a UI-on "A termék törlése sikertelen! Ellenőrizze, hogy nincs-e raktárban ilyen termék!".</t>
+  </si>
+  <si>
+    <t>Sikeres bejelentkezés után látható 3 fül a navigációban. Az alapértelmezett fül tartalmazza a rögzített tárgyak listáját, megjelennek a gombok a lista fölött: Keresés beviteli mező, Elemek száma oldalanként beviteli lista, Hozzáadás, Szűrők törlése, Törlés (inaktív), Áthelyezés (inaktív) lista alatt: Műveleti Napló Letöltése, Címkék Letöltése, Lapozást biztosító fül. Látható a tárgyak és termek kezelése.</t>
+  </si>
+  <si>
+    <t>Keresés</t>
+  </si>
+  <si>
+    <t>Tároló alapján</t>
+  </si>
+  <si>
+    <t>Sikeres szűrés tároló alapján</t>
+  </si>
+  <si>
+    <t>Megfelelően megjelenik az összes adat a szűrés alapján.</t>
+  </si>
+  <si>
+    <t>Tárgynév alapján</t>
+  </si>
+  <si>
+    <t>Kiírt elemek számának beállítása</t>
+  </si>
+  <si>
+    <t>A lista elemeinek kiválasztása a méret beállításához</t>
+  </si>
+  <si>
+    <t>5, 10, 25, 50, 100, 250</t>
+  </si>
+  <si>
+    <t>Megfelelően változik a listázás mérete.</t>
+  </si>
+  <si>
+    <t>Sikeresen kiválaszthatók az elemek.</t>
+  </si>
+  <si>
+    <t>Sikeres szűrés tárgynév alapján.</t>
+  </si>
+  <si>
+    <t>Sikertelen tároló törlés.</t>
+  </si>
+  <si>
+    <t>Sikertelen tárgy törlés.</t>
+  </si>
+  <si>
+    <t>Sikeres tárgynév rögzítés.</t>
+  </si>
+  <si>
+    <t>Sikeres bejelentkezés.</t>
+  </si>
+  <si>
+    <t>Sikeres tároló rögzítés.</t>
+  </si>
+  <si>
+    <t>BZSH-Teszt tárgy-107</t>
+  </si>
+  <si>
+    <t>Termék kód alapján</t>
+  </si>
+  <si>
+    <t>Sikeres szűrés termék kód alapján.</t>
+  </si>
+  <si>
+    <t>Megfelelően megjelenik az egyedi adat a szűrés alapján.</t>
+  </si>
+  <si>
+    <t>Kijelölése a kívánt tárgy(ak)nak</t>
+  </si>
+  <si>
+    <t>A törlés és áthelyezés gombok aktívak lesznek. Megfelelő sikert jelző üzenet jelenik meg a UI-on "A termék(ek) sikeresen áthelyezve!". A listában kiíródik a tárgy az új tároló értékével.</t>
+  </si>
+  <si>
+    <t>A törlés és áthelyezés gombok aktívak lesznek. Megfelelő sikert jelző üzenet jelenik meg a UI-on "A termék(ek) sikeresen törölve!". A listából eltűnik az tárgy.</t>
+  </si>
+  <si>
+    <t>Lapozás</t>
+  </si>
+  <si>
+    <t>A lapozó gombok használata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobbra - Balra </t>
+  </si>
+  <si>
+    <t>A gombok aktívak.</t>
+  </si>
+  <si>
+    <t>Lapozás következtében új elemek töltődnek be.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak.</t>
+  </si>
+  <si>
+    <t>Mégse gomb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megnyílik a modális ablak. </t>
+  </si>
+  <si>
+    <t>Sikeresen megszakad tárgynév törlés. Változatlan a tárgynév lista.</t>
+  </si>
+  <si>
+    <t>Sikeresen megszakad tároló törlés. Változatlan a tároló lista.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. Sikeres tárgy törlés.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. Sikeres tároló törlés.</t>
+  </si>
+  <si>
+    <t>Törlés gomb</t>
+  </si>
+  <si>
+    <t>Áthelyezés gomb</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. Sikeres tárgy áthelyezés.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak sikeres adatkitöltés. Sikeres tárgy rögzítés.</t>
+  </si>
+  <si>
+    <t>Műveleti napló letöltése</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. A szűrőmezők használhatók, kitölthetők.</t>
+  </si>
+  <si>
+    <t>Letöltés gombra letöltődik egy excel file.</t>
+  </si>
+  <si>
+    <t>Műveleti napló szűrői</t>
+  </si>
+  <si>
+    <t>Mégse gombra kattintva a folyamat megszakad, de újra a szűrők betöltve maradnak.</t>
+  </si>
+  <si>
+    <t>Szűrők törlése gombra kattintva a folyamat folytatódik, de a szűrők törlődnek.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. A dátum szűrők tól-ig kitölthetők.</t>
+  </si>
+  <si>
+    <t>Hibás dátumpár pl. 2025-04-01 - 2024-02-02 hibát dob. "Letöltés sikertelen! A záró dátum nem lehet korábbi, mint a kezdő dátum!".</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. A felhasználó szűrő listából választható.</t>
+  </si>
+  <si>
+    <t>NEM Elvárt</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. A tároló szűrő listából választható.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. A tárgynév szűrő listából választható.</t>
+  </si>
+  <si>
+    <t>Címkék</t>
+  </si>
+  <si>
+    <t>Felhasználók navígáció kattintható</t>
+  </si>
+  <si>
+    <t>Megjelennek a felhasználók egy listában a rajtuk alkalmazható funkciókkal. A letiltott felhasználók egy elkülönített listában a rajtuk alkalmazható funkciókkal. A listák felett egy kereső fül.</t>
+  </si>
+  <si>
+    <t>Megnyílik a modális ablak. Kijelölhető az admin tulajdonság. Email kiküldése gomb aktív email megadása után.</t>
+  </si>
+  <si>
+    <t>Megfelelő sikert jelző üzenet jelenik meg a UI-on  "Email kiküldve!".</t>
+  </si>
+  <si>
+    <t>Felhasználó felvitel</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>example@email.com</t>
+  </si>
+  <si>
+    <t>Létező e-maillel tesztelhető kizárólag, a jelszó csak onnan érhető el.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +359,32 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,8 +414,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -215,12 +469,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -264,9 +582,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -276,10 +591,61 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Hivatkozás" xfId="3" builtinId="8"/>
     <cellStyle name="Jó" xfId="1" builtinId="26"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Rossz" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -557,26 +923,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:K15"/>
+  <dimension ref="C7:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="20" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="3:11" s="2" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="18" t="s">
-        <v>18</v>
+      <c r="C8" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>0</v>
@@ -600,11 +968,11 @@
         <v>2</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" s="1" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" s="1" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="17">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -619,94 +987,1012 @@
       <c r="G9" s="5"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="12" t="s">
-        <v>6</v>
+      <c r="J9" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" ht="253.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="18"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="304.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="17"/>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+      <c r="J10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="17">
         <v>2</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="12" t="s">
-        <v>14</v>
+      <c r="J11" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="18"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="79.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
       <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+      <c r="J12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="17">
         <v>3</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="3:11" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
       <c r="D14" s="8"/>
       <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="17">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" ht="87.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="16">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="17">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" ht="129.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="17">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" ht="123.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="17"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="17">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" ht="89.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="17"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="17">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="17"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="17">
+        <v>9</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="17"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="17">
+        <v>10</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="65.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="17"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="17">
+        <v>11</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="17"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="17">
+        <v>12</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="17"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="17">
+        <v>13</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="17"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="17">
+        <v>14</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="17"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="17">
+        <v>15</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="17"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="17">
+        <v>16</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="17"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="17">
+        <v>17</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="17"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="17">
+        <v>18</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="17"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="17">
+        <v>19</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="17"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="17">
+        <v>20</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="17"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="17">
+        <v>21</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="17"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="17">
+        <v>22</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K51" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="17"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="17">
+        <v>23</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="17"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+    </row>
+    <row r="55" spans="3:14" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="17">
+        <v>24</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="K55" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="17"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+    </row>
+    <row r="57" spans="3:14" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="17">
+        <v>25</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="K57" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="17"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+    </row>
+    <row r="59" spans="3:14" ht="151.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="17">
+        <v>26</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K59" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="17"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="31"/>
+    </row>
+    <row r="61" spans="3:14" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="17">
+        <v>27</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="K61" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="N61" s="30"/>
+    </row>
+    <row r="62" spans="3:14" ht="44.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="17"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K62" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F13:F14"/>
+  <mergeCells count="7">
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="E17:G18"/>
+    <mergeCell ref="E19:G20"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F21:F22"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E62" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>